<commit_message>
Update minigame background and icons
</commit_message>
<xml_diff>
--- a/result/results.xlsx
+++ b/result/results.xlsx
@@ -1,42 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\New folder\result\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DECD1B-2F98-472C-BA27-D6CEBB9A91EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -55,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -369,20 +419,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.9296875" customWidth="1"/>
-    <col min="3" max="3" width="28.3984375" customWidth="1"/>
+    <col width="26.33203125" customWidth="1" min="1" max="1"/>
+    <col width="20.9296875" customWidth="1" min="2" max="2"/>
+    <col width="28.3984375" customWidth="1" min="3" max="3"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Mon_Dec__4_07_13_32_2023</t>
+        </is>
+      </c>
+      <c r="C1" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Mon_Dec__4_07_17_55_2023</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Items interact with characters
</commit_message>
<xml_diff>
--- a/result/results.xlsx
+++ b/result/results.xlsx
@@ -1,42 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\New folder\result\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23951FD-8EF3-4111-8091-C36C32C2BB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="3472" windowWidth="16200" windowHeight="9308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4290" yWindow="3472" windowWidth="16200" windowHeight="9308" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -55,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -369,20 +419,130 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G9" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.9296875" customWidth="1"/>
-    <col min="3" max="3" width="28.3984375" customWidth="1"/>
+    <col width="26.33203125" customWidth="1" min="1" max="1"/>
+    <col width="20.9296875" customWidth="1" min="2" max="2"/>
+    <col width="28.3984375" customWidth="1" min="3" max="3"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Mon_Dec__4_15_55_04_2023</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="C1" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Mon_Dec__4_16_06_35_2023</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Mon_Dec__4_16_09_58_2023</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Mon_Dec__4_16_12_03_2023</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Mon_Dec__4_16_16_40_2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Mon_Dec__4_16_16_43_2023</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Mon_Dec__4_16_17_36_2023</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix wrong restart coordiate in Car class && Stop ani when finish
</commit_message>
<xml_diff>
--- a/result/results.xlsx
+++ b/result/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="A1:C14"/>
@@ -467,6 +467,36 @@
         <v>30</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Tue_Dec__5_09_17_31_2023</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Tue_Dec__5_09_20_16_2023</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added player set 2
</commit_message>
<xml_diff>
--- a/result/results.xlsx
+++ b/result/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="A1:C14"/>
@@ -512,6 +512,36 @@
         <v>30</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Tue_Dec__5_12_34_52_2023</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Tue_Dec__5_12_37_31_2023</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added characters set 4
</commit_message>
<xml_diff>
--- a/result/results.xlsx
+++ b/result/results.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G8" sqref="A1:XFD1048576"/>
@@ -452,6 +452,21 @@
         <v>30</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Thu_Dec__7_18_18_59_2023</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated characters set 4
</commit_message>
<xml_diff>
--- a/result/results.xlsx
+++ b/result/results.xlsx
@@ -1,33 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\New folder\result\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99794F62-2EC3-47A5-AC9D-9E969878C066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="3195" yWindow="2348" windowWidth="16200" windowHeight="9307" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>Coin</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -45,81 +72,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -419,55 +388,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="A1:XFD1048576"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col width="26.33203125" customWidth="1" min="1" max="1"/>
-    <col width="20.9296875" customWidth="1" min="2" max="2"/>
-    <col width="28.3984375" customWidth="1" min="3" max="3"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.9296875" customWidth="1"/>
+    <col min="3" max="3" width="28.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Wed_Dec__6_07_33_35_2023</t>
-        </is>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>f</t>
-        </is>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
-      <c r="C1" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Thu_Dec__7_18_18_59_2023</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>f</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>30</v>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Buttons behavior base on login state
</commit_message>
<xml_diff>
--- a/result/results.xlsx
+++ b/result/results.xlsx
@@ -1,41 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\New folder\result\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DCEA00-0957-4F00-8255-9538ACB52E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>Coin</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -54,81 +73,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -428,174 +388,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="A2:F16"/>
+      <selection activeCell="F13" sqref="A2:F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col width="26.33203125" customWidth="1" min="1" max="1"/>
-    <col width="20.9296875" customWidth="1" min="2" max="2"/>
-    <col width="28.3984375" customWidth="1" min="3" max="3"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.9296875" customWidth="1"/>
+    <col min="3" max="3" width="28.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Time</t>
-        </is>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Player</t>
-        </is>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Coin</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Sun Dec 17 00_23_02 2023</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>loc</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Sun Dec 17 00_26_18 2023</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>loc</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Sun Dec 17 00_41_36 2023</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>loc</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Sun Dec 17 00_46_58 2023</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>loc</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Sun Dec 17 00_52_41 2023</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>loc</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Sun Dec 17 03_25_16 2023</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>loc</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Sun Dec 17 03_26_53 2023</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>loc</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Sun Dec 17 03_29_21 2023</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>loc</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Sun Dec 17 03_31_50 2023</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>loc</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>180</v>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>